<commit_message>
first architecture check with jochen on friday, 10_06_2016
</commit_message>
<xml_diff>
--- a/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Architektur.xlsx
+++ b/docs/documentation/Qualitätsmanagement/Checklisten/Checkliste_Architektur.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Checkliste Architekturdokument</t>
   </si>
@@ -67,14 +67,34 @@
   </si>
   <si>
     <t>erklärende Diagramme vorhanden?</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>ja, angepasst</t>
+  </si>
+  <si>
+    <t>wird gestrichen</t>
+  </si>
+  <si>
+    <t>gecheckt am 10.06.2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -102,8 +122,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -398,105 +419,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C19"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:3">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:3">
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
       <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:3">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
       <c r="C8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:3">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
       <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:3">
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
       <c r="B10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:3">
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
       <c r="C11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="2:3">
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
       <c r="C12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="2:3">
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
       <c r="C13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="2:3">
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
       <c r="B14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="2:3">
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
       <c r="B15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:3">
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
       <c r="B16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="2:2">
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:2">
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="2:2">
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" t="s">
         <v>14</v>
       </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="77" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>